<commit_message>
remove spaces from string end (warning unit test) 4e36680a742783a3bf8aef10e4f6c671dad0f595
</commit_message>
<xml_diff>
--- a/ig/majKereval/StructureDefinition-ror-healthcareservice.xlsx
+++ b/ig/majKereval/StructureDefinition-ror-healthcareservice.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-11T08:38:10+00:00</t>
+    <t>2023-04-11T08:56:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Profil créé dans le cadre du ROR pour décrire les prestations que peut réaliser une structure et qui permettent de répondre au besoin de santé d'une personne </t>
+    <t>Profil créé dans le cadre du ROR pour décrire les prestations que peut réaliser une structure et qui permettent de répondre au besoin de santé d'une personne</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -1062,7 +1062,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">utilisation (Telecommunication) : Utilisation du canal de communication </t>
+    <t>utilisation (Telecommunication) : Utilisation du canal de communication</t>
   </si>
   <si>
     <t xml:space="preserve">Extension créée dans le cadre du ROR qui précise l'utilisation du canal de communication </t>
@@ -1458,7 +1458,7 @@
     <t>expertiseLevel</t>
   </si>
   <si>
-    <t xml:space="preserve">niveauExpertise (OffreOperationnelle) : Niveau de ressources humaines et matérielles engagées dans la réalisation de l'offre </t>
+    <t>niveauExpertise (OffreOperationnelle) : Niveau de ressources humaines et matérielles engagées dans la réalisation de l'offre</t>
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J227-NiveauExpertise-ROR/FHIR/JDV-J227-NiveauExpertise-ROR</t>

</xml_diff>